<commit_message>
Added new meta type tkMetaType
</commit_message>
<xml_diff>
--- a/tests/docsrc/tables.xlsx
+++ b/tests/docsrc/tables.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\metapp\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\metapp\tests\docsrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B66FBDE-2065-4D2D-9CF9-658C1749AE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4EBD57-0A0A-40F5-8186-053977782F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="147">
   <si>
     <t>TypeKind</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -590,6 +590,14 @@
   <si>
     <t>MetaAccessible
 MetaMember</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tkMetaType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>metapp::MetaType</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -919,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1397,27 +1405,24 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>66</v>
+        <v>145</v>
       </c>
       <c r="B32">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="C32" t="s">
-        <v>101</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B33">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -1425,30 +1430,27 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B34">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E34">
-        <v>1</v>
-      </c>
-      <c r="F34" t="s">
-        <v>104</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B35">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C35" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -1457,55 +1459,52 @@
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36">
+        <v>73</v>
+      </c>
+      <c r="C36" t="s">
+        <v>108</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>70</v>
       </c>
-      <c r="B36">
+      <c r="B37">
         <v>74</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>109</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>115</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E37" t="s">
         <v>49</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B37">
-        <v>75</v>
-      </c>
-      <c r="C37" t="s">
-        <v>110</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-      <c r="F37" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B38">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C38" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>118</v>
@@ -1519,13 +1518,13 @@
     </row>
     <row r="39" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B39">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>118</v>
@@ -1539,13 +1538,13 @@
     </row>
     <row r="40" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B40">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C40" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>118</v>
@@ -1557,18 +1556,18 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B41">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C41" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -1579,27 +1578,33 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B42">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C42" t="s">
-        <v>122</v>
+        <v>120</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F42" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B43">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -1607,47 +1612,41 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44">
+        <v>81</v>
+      </c>
+      <c r="C44" t="s">
+        <v>123</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>78</v>
       </c>
-      <c r="B44">
+      <c r="B45">
         <v>82</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>124</v>
       </c>
-      <c r="E44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="E45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>79</v>
       </c>
-      <c r="B45">
+      <c r="B46">
         <v>83</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>125</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E45">
-        <v>2</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>80</v>
-      </c>
-      <c r="B46">
-        <v>84</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>142</v>
@@ -1659,35 +1658,35 @@
         <v>126</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>80</v>
+      </c>
+      <c r="B47">
+        <v>84</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>81</v>
       </c>
-      <c r="B47">
+      <c r="B48">
         <v>85</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>127</v>
-      </c>
-      <c r="D47" t="s">
-        <v>121</v>
-      </c>
-      <c r="E47">
-        <v>1</v>
-      </c>
-      <c r="F47" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="69" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>82</v>
-      </c>
-      <c r="B48">
-        <v>86</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="D48" t="s">
         <v>121</v>
@@ -1699,35 +1698,35 @@
         <v>128</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="96.6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="69" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B49">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
+      </c>
+      <c r="D49" t="s">
+        <v>121</v>
       </c>
       <c r="E49">
-        <v>2</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>126</v>
+        <v>1</v>
+      </c>
+      <c r="F49" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="96.6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B50">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>142</v>
@@ -1739,35 +1738,35 @@
         <v>126</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="96.6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B51">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D51" t="s">
-        <v>121</v>
+        <v>138</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="E51">
-        <v>1</v>
-      </c>
-      <c r="F51" t="s">
-        <v>128</v>
+        <v>2</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B52">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D52" t="s">
         <v>121</v>
@@ -1779,82 +1778,102 @@
         <v>128</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B53">
-        <v>91</v>
-      </c>
-      <c r="C53" t="s">
-        <v>129</v>
+        <v>90</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="D53" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="E53">
         <v>1</v>
       </c>
-      <c r="F53" s="1" t="s">
+      <c r="F53" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>87</v>
+      </c>
+      <c r="B54">
+        <v>91</v>
+      </c>
+      <c r="C54" t="s">
+        <v>129</v>
+      </c>
+      <c r="D54" t="s">
+        <v>117</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="55" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>88</v>
       </c>
-      <c r="B54">
+      <c r="B55">
         <v>92</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>131</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E55" t="s">
         <v>132</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="F55" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>89</v>
       </c>
-      <c r="B55">
+      <c r="B56">
         <v>93</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" t="s">
         <v>134</v>
       </c>
-      <c r="E55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="E56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>90</v>
       </c>
-      <c r="B56">
+      <c r="B57">
         <v>94</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>135</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E57" t="s">
         <v>132</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="F57" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>91</v>
       </c>
-      <c r="B57">
+      <c r="B58">
         <v>1024</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new meta type tkOverloadedFunction
</commit_message>
<xml_diff>
--- a/tests/docsrc/tables.xlsx
+++ b/tests/docsrc/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\metapp\tests\docsrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4EBD57-0A0A-40F5-8186-053977782F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8937D9-F339-4738-A6EB-A0CB4CC95957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="150">
   <si>
     <t>TypeKind</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -598,6 +598,18 @@
   </si>
   <si>
     <t>metapp::MetaType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tkMetaRepo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>metapp::MetaRepo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tkOverloadedFunction</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -927,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1315,7 +1327,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>97</v>
+        <v>149</v>
       </c>
       <c r="B26">
         <v>37</v>
@@ -1323,13 +1335,11 @@
       <c r="D26" t="s">
         <v>115</v>
       </c>
-      <c r="E26" t="s">
-        <v>96</v>
-      </c>
+      <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>97</v>
       </c>
       <c r="B27">
         <v>38</v>
@@ -1337,177 +1347,162 @@
       <c r="D27" t="s">
         <v>115</v>
       </c>
-      <c r="E27">
-        <v>0</v>
+      <c r="E27" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B28">
         <v>39</v>
       </c>
       <c r="D28" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E28">
-        <v>1</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>105</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B29">
         <v>40</v>
       </c>
+      <c r="D29" t="s">
+        <v>117</v>
+      </c>
       <c r="E29">
         <v>1</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="B30">
         <v>41</v>
       </c>
-      <c r="D30" t="s">
-        <v>114</v>
-      </c>
       <c r="E30">
         <v>1</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B31">
         <v>42</v>
       </c>
-      <c r="C31" t="s">
-        <v>100</v>
+      <c r="D31" t="s">
+        <v>114</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>145</v>
+        <v>65</v>
       </c>
       <c r="B32">
         <v>43</v>
       </c>
       <c r="C32" t="s">
-        <v>146</v>
+        <v>100</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>145</v>
       </c>
       <c r="B33">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="C33" t="s">
-        <v>101</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>67</v>
+        <v>147</v>
       </c>
       <c r="B34">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="C34" t="s">
-        <v>102</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B35">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C35" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E35">
-        <v>1</v>
-      </c>
-      <c r="F35" t="s">
-        <v>104</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36">
+        <v>71</v>
+      </c>
+      <c r="C36" t="s">
+        <v>102</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37">
+        <v>72</v>
+      </c>
+      <c r="C37" t="s">
+        <v>103</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>69</v>
       </c>
-      <c r="B36">
+      <c r="B38">
         <v>73</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C38" t="s">
         <v>108</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="F36" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37">
-        <v>74</v>
-      </c>
-      <c r="C37" t="s">
-        <v>109</v>
-      </c>
-      <c r="D37" t="s">
-        <v>115</v>
-      </c>
-      <c r="E37" t="s">
-        <v>49</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>71</v>
-      </c>
-      <c r="B38">
-        <v>75</v>
-      </c>
-      <c r="C38" t="s">
-        <v>110</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -1516,35 +1511,35 @@
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B39">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C39" t="s">
-        <v>111</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="F39" t="s">
-        <v>104</v>
+        <v>109</v>
+      </c>
+      <c r="D39" t="s">
+        <v>115</v>
+      </c>
+      <c r="E39" t="s">
+        <v>49</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B40">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C40" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>118</v>
@@ -1558,13 +1553,13 @@
     </row>
     <row r="41" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B41">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C41" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>118</v>
@@ -1576,18 +1571,18 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B42">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C42" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E42">
         <v>1</v>
@@ -1596,271 +1591,280 @@
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B43">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C43" t="s">
-        <v>122</v>
+        <v>119</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F43" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B44">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C44" t="s">
-        <v>123</v>
+        <v>120</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F44" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45">
+        <v>80</v>
+      </c>
+      <c r="C45" t="s">
+        <v>122</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46">
+        <v>81</v>
+      </c>
+      <c r="C46" t="s">
+        <v>123</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>78</v>
       </c>
-      <c r="B45">
+      <c r="B47">
         <v>82</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C47" t="s">
         <v>124</v>
       </c>
-      <c r="E45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="E47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>79</v>
       </c>
-      <c r="B46">
+      <c r="B48">
         <v>83</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C48" t="s">
         <v>125</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E46">
+      <c r="E48">
         <v>2</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="49" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>80</v>
       </c>
-      <c r="B47">
+      <c r="B49">
         <v>84</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E47">
+      <c r="E49">
         <v>2</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>81</v>
       </c>
-      <c r="B48">
+      <c r="B50">
         <v>85</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C50" t="s">
         <v>127</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D50" t="s">
         <v>121</v>
       </c>
-      <c r="E48">
+      <c r="E50">
         <v>1</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F50" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="69" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="51" spans="1:6" ht="69" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>82</v>
       </c>
-      <c r="B49">
+      <c r="B51">
         <v>86</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D51" t="s">
         <v>121</v>
       </c>
-      <c r="E49">
+      <c r="E51">
         <v>1</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F51" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="96.6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="52" spans="1:6" ht="96.6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>83</v>
       </c>
-      <c r="B50">
+      <c r="B52">
         <v>87</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E50">
+      <c r="E52">
         <v>2</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="F52" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="96.6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="53" spans="1:6" ht="96.6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>84</v>
       </c>
-      <c r="B51">
+      <c r="B53">
         <v>88</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E51">
+      <c r="E53">
         <v>2</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="F53" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="54" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>85</v>
       </c>
-      <c r="B52">
+      <c r="B54">
         <v>89</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D54" t="s">
         <v>121</v>
-      </c>
-      <c r="E52">
-        <v>1</v>
-      </c>
-      <c r="F52" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>86</v>
-      </c>
-      <c r="B53">
-        <v>90</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D53" t="s">
-        <v>121</v>
-      </c>
-      <c r="E53">
-        <v>1</v>
-      </c>
-      <c r="F53" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>87</v>
-      </c>
-      <c r="B54">
-        <v>91</v>
-      </c>
-      <c r="C54" t="s">
-        <v>129</v>
-      </c>
-      <c r="D54" t="s">
-        <v>117</v>
       </c>
       <c r="E54">
         <v>1</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="F54" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>86</v>
+      </c>
+      <c r="B55">
+        <v>90</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D55" t="s">
+        <v>121</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>87</v>
+      </c>
+      <c r="B56">
+        <v>91</v>
+      </c>
+      <c r="C56" t="s">
+        <v>129</v>
+      </c>
+      <c r="D56" t="s">
+        <v>117</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>88</v>
-      </c>
-      <c r="B55">
-        <v>92</v>
-      </c>
-      <c r="C55" t="s">
-        <v>131</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E55" t="s">
-        <v>132</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>89</v>
-      </c>
-      <c r="B56">
-        <v>93</v>
-      </c>
-      <c r="C56" t="s">
-        <v>134</v>
-      </c>
-      <c r="E56">
-        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B57">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C57" t="s">
-        <v>135</v>
+        <v>131</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="E57" t="s">
         <v>132</v>
@@ -1871,9 +1875,40 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>89</v>
+      </c>
+      <c r="B58">
+        <v>93</v>
+      </c>
+      <c r="C58" t="s">
+        <v>134</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>90</v>
+      </c>
+      <c r="B59">
+        <v>94</v>
+      </c>
+      <c r="C59" t="s">
+        <v>135</v>
+      </c>
+      <c r="E59" t="s">
+        <v>132</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>91</v>
       </c>
-      <c r="B58">
+      <c r="B60">
         <v>1024</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed MetaAccessible interface from pointer and member data pointer, because that's too general and overkill. Now limit MetaAccessible to Accessor
</commit_message>
<xml_diff>
--- a/tests/docsrc/tables.xlsx
+++ b/tests/docsrc/tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\metapp\tests\docsrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8937D9-F339-4738-A6EB-A0CB4CC95957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3EB9EAA-5130-49F6-B05E-DC8036EB6E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="149">
   <si>
     <t>TypeKind</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -584,15 +584,6 @@
 MetaMappable</t>
   </si>
   <si>
-    <t>MetaAccessible</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MetaAccessible
-MetaMember</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>tkMetaType</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -610,6 +601,10 @@
   </si>
   <si>
     <t>tkOverloadedFunction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MetaMember</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -942,7 +937,7 @@
   <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1230,9 +1225,6 @@
       <c r="C20" t="s">
         <v>98</v>
       </c>
-      <c r="D20" t="s">
-        <v>143</v>
-      </c>
       <c r="E20">
         <v>1</v>
       </c>
@@ -1299,7 +1291,7 @@
         <v>35</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="E24">
         <v>2</v>
@@ -1327,7 +1319,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B26">
         <v>37</v>
@@ -1429,24 +1421,24 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B33">
         <v>44</v>
       </c>
       <c r="C33" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B34">
         <v>45</v>
       </c>
       <c r="C34" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed type kind values
</commit_message>
<xml_diff>
--- a/tests/docsrc/tables.xlsx
+++ b/tests/docsrc/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\metapp\tests\docsrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335718BE-3AFE-41CE-A4EE-265357C56ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5917669A-29C1-413F-ACB3-12F64A010790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="150">
   <si>
     <t>TypeKind</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -584,40 +584,30 @@
 MetaMappable</t>
   </si>
   <si>
+    <t>tkOverloadedFunction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MetaMember</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tkChar8 (C++20)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tkChar16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tkChar32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>tkMetaType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>metapp::MetaType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>tkMetaRepo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>metapp::MetaRepo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tkOverloadedFunction</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MetaMember</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tkChar8 (C++20)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tkChar16</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tkChar32</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -948,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1039,7 +1029,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -1047,7 +1037,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -1055,7 +1045,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -1248,7 +1238,7 @@
         <v>37</v>
       </c>
       <c r="B22">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1256,7 +1246,7 @@
         <v>38</v>
       </c>
       <c r="B23">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
         <v>98</v>
@@ -1273,7 +1263,7 @@
         <v>39</v>
       </c>
       <c r="B24">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C24" t="s">
         <v>99</v>
@@ -1290,7 +1280,7 @@
         <v>40</v>
       </c>
       <c r="B25">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D25" t="s">
         <v>115</v>
@@ -1307,7 +1297,7 @@
         <v>41</v>
       </c>
       <c r="B26">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>116</v>
@@ -1324,10 +1314,10 @@
         <v>42</v>
       </c>
       <c r="B27">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E27">
         <v>2</v>
@@ -1341,7 +1331,7 @@
         <v>43</v>
       </c>
       <c r="B28">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>116</v>
@@ -1355,10 +1345,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B29">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D29" t="s">
         <v>115</v>
@@ -1370,7 +1360,7 @@
         <v>97</v>
       </c>
       <c r="B30">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D30" t="s">
         <v>115</v>
@@ -1384,7 +1374,7 @@
         <v>46</v>
       </c>
       <c r="B31">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D31" t="s">
         <v>115</v>
@@ -1398,7 +1388,7 @@
         <v>44</v>
       </c>
       <c r="B32">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D32" t="s">
         <v>117</v>
@@ -1415,7 +1405,7 @@
         <v>45</v>
       </c>
       <c r="B33">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -1429,7 +1419,7 @@
         <v>64</v>
       </c>
       <c r="B34">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="D34" t="s">
         <v>114</v>
@@ -1446,7 +1436,7 @@
         <v>65</v>
       </c>
       <c r="B35">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C35" t="s">
         <v>100</v>
@@ -1457,24 +1447,18 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="B36">
-        <v>44</v>
-      </c>
-      <c r="C36" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B37">
-        <v>45</v>
-      </c>
-      <c r="C37" t="s">
-        <v>146</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1482,7 +1466,7 @@
         <v>66</v>
       </c>
       <c r="B38">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="C38" t="s">
         <v>101</v>
@@ -1496,7 +1480,7 @@
         <v>67</v>
       </c>
       <c r="B39">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="C39" t="s">
         <v>102</v>
@@ -1510,7 +1494,7 @@
         <v>68</v>
       </c>
       <c r="B40">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="C40" t="s">
         <v>103</v>
@@ -1527,7 +1511,7 @@
         <v>69</v>
       </c>
       <c r="B41">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="C41" t="s">
         <v>108</v>
@@ -1544,7 +1528,7 @@
         <v>70</v>
       </c>
       <c r="B42">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="C42" t="s">
         <v>109</v>
@@ -1564,7 +1548,7 @@
         <v>71</v>
       </c>
       <c r="B43">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="C43" t="s">
         <v>110</v>
@@ -1584,7 +1568,7 @@
         <v>72</v>
       </c>
       <c r="B44">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="C44" t="s">
         <v>111</v>
@@ -1604,7 +1588,7 @@
         <v>73</v>
       </c>
       <c r="B45">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="C45" t="s">
         <v>112</v>
@@ -1624,7 +1608,7 @@
         <v>74</v>
       </c>
       <c r="B46">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="C46" t="s">
         <v>119</v>
@@ -1644,7 +1628,7 @@
         <v>75</v>
       </c>
       <c r="B47">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="C47" t="s">
         <v>120</v>
@@ -1664,7 +1648,7 @@
         <v>76</v>
       </c>
       <c r="B48">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="C48" t="s">
         <v>122</v>
@@ -1678,7 +1662,7 @@
         <v>77</v>
       </c>
       <c r="B49">
-        <v>81</v>
+        <v>111</v>
       </c>
       <c r="C49" t="s">
         <v>123</v>
@@ -1692,7 +1676,7 @@
         <v>78</v>
       </c>
       <c r="B50">
-        <v>82</v>
+        <v>112</v>
       </c>
       <c r="C50" t="s">
         <v>124</v>
@@ -1706,7 +1690,7 @@
         <v>79</v>
       </c>
       <c r="B51">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="C51" t="s">
         <v>125</v>
@@ -1726,7 +1710,7 @@
         <v>80</v>
       </c>
       <c r="B52">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>141</v>
@@ -1746,7 +1730,7 @@
         <v>81</v>
       </c>
       <c r="B53">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="C53" t="s">
         <v>127</v>
@@ -1766,7 +1750,7 @@
         <v>82</v>
       </c>
       <c r="B54">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>140</v>
@@ -1786,7 +1770,7 @@
         <v>83</v>
       </c>
       <c r="B55">
-        <v>87</v>
+        <v>117</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>139</v>
@@ -1806,7 +1790,7 @@
         <v>84</v>
       </c>
       <c r="B56">
-        <v>88</v>
+        <v>118</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>138</v>
@@ -1826,7 +1810,7 @@
         <v>85</v>
       </c>
       <c r="B57">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>137</v>
@@ -1846,7 +1830,7 @@
         <v>86</v>
       </c>
       <c r="B58">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>136</v>
@@ -1866,7 +1850,7 @@
         <v>87</v>
       </c>
       <c r="B59">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="C59" t="s">
         <v>129</v>
@@ -1886,7 +1870,7 @@
         <v>88</v>
       </c>
       <c r="B60">
-        <v>92</v>
+        <v>122</v>
       </c>
       <c r="C60" t="s">
         <v>131</v>
@@ -1906,7 +1890,7 @@
         <v>89</v>
       </c>
       <c r="B61">
-        <v>93</v>
+        <v>123</v>
       </c>
       <c r="C61" t="s">
         <v>134</v>
@@ -1920,7 +1904,7 @@
         <v>90</v>
       </c>
       <c r="B62">
-        <v>94</v>
+        <v>124</v>
       </c>
       <c r="C62" t="s">
         <v>135</v>

</xml_diff>

<commit_message>
Added MetaAccessible interface back to pointer and member data pointer
</commit_message>
<xml_diff>
--- a/tests/docsrc/tables.xlsx
+++ b/tests/docsrc/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\metapp\tests\docsrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5917669A-29C1-413F-ACB3-12F64A010790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFB35D6-67F7-4119-AA26-25DE1627107B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="151">
   <si>
     <t>TypeKind</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -588,10 +588,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MetaMember</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>tkChar8 (C++20)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -608,6 +604,14 @@
   </si>
   <si>
     <t>tkMetaRepo</t>
+  </si>
+  <si>
+    <t>MetaAccessible</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MetaAccessible</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -938,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1029,7 +1033,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -1037,7 +1041,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -1045,7 +1049,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -1251,6 +1255,9 @@
       <c r="C23" t="s">
         <v>98</v>
       </c>
+      <c r="D23" t="s">
+        <v>150</v>
+      </c>
       <c r="E23">
         <v>1</v>
       </c>
@@ -1300,7 +1307,7 @@
         <v>44</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E26" t="s">
         <v>50</v>
@@ -1317,7 +1324,7 @@
         <v>45</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="E27">
         <v>2</v>
@@ -1447,7 +1454,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B36">
         <v>54</v>
@@ -1455,7 +1462,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B37">
         <v>55</v>

</xml_diff>

<commit_message>
Added meta type for std::weak_ptr
</commit_message>
<xml_diff>
--- a/tests/docsrc/tables.xlsx
+++ b/tests/docsrc/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\metapp\tests\docsrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFB35D6-67F7-4119-AA26-25DE1627107B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F7FBDD-E9AD-44F1-AB57-7D304F4017EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="154">
   <si>
     <t>TypeKind</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -611,6 +611,18 @@
   </si>
   <si>
     <t>MetaAccessible</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tkStdWeakPtr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>std::weak_ptr&lt;T&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -940,10 +952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1530,55 +1542,52 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>70</v>
+        <v>151</v>
       </c>
       <c r="B42">
         <v>104</v>
       </c>
       <c r="C42" t="s">
-        <v>109</v>
-      </c>
-      <c r="D42" t="s">
-        <v>115</v>
-      </c>
-      <c r="E42" t="s">
-        <v>49</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B43">
         <v>105</v>
       </c>
       <c r="C43" t="s">
-        <v>110</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E43">
-        <v>1</v>
-      </c>
-      <c r="F43" t="s">
-        <v>104</v>
+        <v>109</v>
+      </c>
+      <c r="D43" t="s">
+        <v>115</v>
+      </c>
+      <c r="E43" t="s">
+        <v>49</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B44">
         <v>106</v>
       </c>
       <c r="C44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>118</v>
@@ -1592,13 +1601,13 @@
     </row>
     <row r="45" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B45">
         <v>107</v>
       </c>
       <c r="C45" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>118</v>
@@ -1612,13 +1621,13 @@
     </row>
     <row r="46" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B46">
         <v>108</v>
       </c>
       <c r="C46" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>118</v>
@@ -1630,18 +1639,18 @@
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B47">
         <v>109</v>
       </c>
       <c r="C47" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -1652,27 +1661,33 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B48">
         <v>110</v>
       </c>
       <c r="C48" t="s">
-        <v>122</v>
+        <v>120</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F48" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B49">
         <v>111</v>
       </c>
       <c r="C49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E49">
         <v>0</v>
@@ -1680,47 +1695,41 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B50">
         <v>112</v>
       </c>
       <c r="C50" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E50">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B51">
         <v>113</v>
       </c>
       <c r="C51" t="s">
-        <v>125</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="E51">
-        <v>2</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B52">
         <v>114</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>141</v>
+      <c r="C52" t="s">
+        <v>125</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>142</v>
@@ -1732,35 +1741,35 @@
         <v>126</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B53">
         <v>115</v>
       </c>
-      <c r="C53" t="s">
-        <v>127</v>
-      </c>
-      <c r="D53" t="s">
-        <v>121</v>
+      <c r="C53" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="E53">
-        <v>1</v>
-      </c>
-      <c r="F53" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="69" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B54">
         <v>116</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>140</v>
+      <c r="C54" t="s">
+        <v>127</v>
       </c>
       <c r="D54" t="s">
         <v>121</v>
@@ -1772,35 +1781,35 @@
         <v>128</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="96.6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="69" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B55">
         <v>117</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
+      </c>
+      <c r="D55" t="s">
+        <v>121</v>
       </c>
       <c r="E55">
-        <v>2</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>126</v>
+        <v>1</v>
+      </c>
+      <c r="F55" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="96.6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B56">
         <v>118</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>142</v>
@@ -1812,35 +1821,35 @@
         <v>126</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="96.6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B57">
         <v>119</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D57" t="s">
-        <v>121</v>
+        <v>138</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="E57">
-        <v>1</v>
-      </c>
-      <c r="F57" t="s">
-        <v>128</v>
+        <v>2</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B58">
         <v>120</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D58" t="s">
         <v>121</v>
@@ -1852,82 +1861,102 @@
         <v>128</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B59">
         <v>121</v>
       </c>
-      <c r="C59" t="s">
-        <v>129</v>
+      <c r="C59" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="D59" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="E59">
         <v>1</v>
       </c>
-      <c r="F59" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="F59" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B60">
         <v>122</v>
       </c>
       <c r="C60" t="s">
-        <v>131</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E60" t="s">
-        <v>132</v>
+        <v>129</v>
+      </c>
+      <c r="D60" t="s">
+        <v>117</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B61">
         <v>123</v>
       </c>
       <c r="C61" t="s">
-        <v>134</v>
-      </c>
-      <c r="E61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E61" t="s">
+        <v>132</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B62">
         <v>124</v>
       </c>
       <c r="C62" t="s">
+        <v>134</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>90</v>
+      </c>
+      <c r="B63">
+        <v>125</v>
+      </c>
+      <c r="C63" t="s">
         <v>135</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E63" t="s">
         <v>132</v>
       </c>
-      <c r="F62" s="1" t="s">
+      <c r="F63" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>91</v>
       </c>
-      <c r="B63">
+      <c r="B64">
         <v>1024</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added tool to generate markdown tables from Excel file
</commit_message>
<xml_diff>
--- a/tests/docsrc/tables.xlsx
+++ b/tests/docsrc/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\metapp\tests\docsrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F7FBDD-E9AD-44F1-AB57-7D304F4017EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73BC5DFA-C6B2-48B2-A947-7C2D3D9BC272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="164">
   <si>
     <t>TypeKind</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -623,6 +623,50 @@
   </si>
   <si>
     <t>T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cast to</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>All arithmetic types.
+Any types that can cast arithmetic types to.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ditto</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Any pointers.
+char * can cast to std::string.
+wchar_t * can cast to std::wstring.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use the cast rules of Variant</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>char *</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wchar_t *</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T *
+std::weak_ptr&lt;T&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T *</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>std::shared_ptr&lt;T&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -952,22 +996,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="27.109375" customWidth="1"/>
     <col min="3" max="3" width="57" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" customWidth="1"/>
-    <col min="6" max="6" width="29.5546875" customWidth="1"/>
+    <col min="4" max="4" width="50.44140625" customWidth="1"/>
+    <col min="5" max="5" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
+    <col min="7" max="7" width="29.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -978,16 +1023,19 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1" t="s">
         <v>113</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -997,11 +1045,11 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1011,11 +1059,14 @@
       <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1025,11 +1076,14 @@
       <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1039,35 +1093,47 @@
       <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>144</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>145</v>
       </c>
       <c r="B7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>146</v>
       </c>
       <c r="B8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1077,11 +1143,14 @@
       <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>156</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1091,11 +1160,14 @@
       <c r="C10" t="s">
         <v>24</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>156</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1105,11 +1177,14 @@
       <c r="C11" t="s">
         <v>25</v>
       </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>156</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1119,11 +1194,14 @@
       <c r="C12" t="s">
         <v>26</v>
       </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>156</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1133,11 +1211,14 @@
       <c r="C13" t="s">
         <v>27</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>156</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1147,11 +1228,14 @@
       <c r="C14" t="s">
         <v>28</v>
       </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>156</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1161,11 +1245,14 @@
       <c r="C15" t="s">
         <v>29</v>
       </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>156</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1175,11 +1262,14 @@
       <c r="C16" t="s">
         <v>30</v>
       </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>156</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1189,11 +1279,14 @@
       <c r="C17" t="s">
         <v>31</v>
       </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>156</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1203,11 +1296,14 @@
       <c r="C18" t="s">
         <v>32</v>
       </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>156</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1217,11 +1313,14 @@
       <c r="C19" t="s">
         <v>33</v>
       </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>156</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1231,11 +1330,14 @@
       <c r="C20" t="s">
         <v>34</v>
       </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>156</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1245,11 +1347,14 @@
       <c r="C21" t="s">
         <v>35</v>
       </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>156</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -1257,7 +1362,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -1267,17 +1372,20 @@
       <c r="C23" t="s">
         <v>98</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E23" t="s">
         <v>150</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>1</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -1287,170 +1395,170 @@
       <c r="C24" t="s">
         <v>99</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>1</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>40</v>
       </c>
       <c r="B25">
         <v>43</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>115</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="69" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="69" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>41</v>
       </c>
       <c r="B26">
         <v>44</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>50</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>42</v>
       </c>
       <c r="B27">
         <v>45</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>2</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>43</v>
       </c>
       <c r="B28">
         <v>46</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>49</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>143</v>
       </c>
       <c r="B29">
         <v>47</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>115</v>
       </c>
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>97</v>
       </c>
       <c r="B30">
         <v>48</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>115</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>46</v>
       </c>
       <c r="B31">
         <v>49</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>115</v>
       </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>44</v>
       </c>
       <c r="B32">
         <v>50</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>117</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>1</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>45</v>
       </c>
       <c r="B33">
         <v>51</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>1</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>64</v>
       </c>
       <c r="B34">
         <v>52</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>114</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>1</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>65</v>
       </c>
@@ -1460,11 +1568,14 @@
       <c r="C35" t="s">
         <v>100</v>
       </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>158</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>147</v>
       </c>
@@ -1472,7 +1583,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>148</v>
       </c>
@@ -1480,7 +1591,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>66</v>
       </c>
@@ -1490,11 +1601,14 @@
       <c r="C38" t="s">
         <v>101</v>
       </c>
-      <c r="E38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>159</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>67</v>
       </c>
@@ -1504,11 +1618,14 @@
       <c r="C39" t="s">
         <v>102</v>
       </c>
-      <c r="E39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>160</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>68</v>
       </c>
@@ -1518,14 +1635,17 @@
       <c r="C40" t="s">
         <v>103</v>
       </c>
-      <c r="E40">
+      <c r="D40" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F40">
         <v>1</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>69</v>
       </c>
@@ -1535,14 +1655,17 @@
       <c r="C41" t="s">
         <v>108</v>
       </c>
-      <c r="E41">
+      <c r="D41" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F41">
         <v>1</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>151</v>
       </c>
@@ -1552,14 +1675,17 @@
       <c r="C42" t="s">
         <v>152</v>
       </c>
-      <c r="E42">
+      <c r="D42" t="s">
+        <v>163</v>
+      </c>
+      <c r="F42">
         <v>1</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>70</v>
       </c>
@@ -1569,17 +1695,17 @@
       <c r="C43" t="s">
         <v>109</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>115</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>49</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>71</v>
       </c>
@@ -1589,17 +1715,17 @@
       <c r="C44" t="s">
         <v>110</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E44">
+      <c r="F44">
         <v>1</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>72</v>
       </c>
@@ -1609,17 +1735,17 @@
       <c r="C45" t="s">
         <v>111</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E45">
+      <c r="F45">
         <v>1</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>73</v>
       </c>
@@ -1629,17 +1755,17 @@
       <c r="C46" t="s">
         <v>112</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E46">
+      <c r="F46">
         <v>1</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>74</v>
       </c>
@@ -1649,17 +1775,17 @@
       <c r="C47" t="s">
         <v>119</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E47">
+      <c r="F47">
         <v>1</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>75</v>
       </c>
@@ -1669,17 +1795,17 @@
       <c r="C48" t="s">
         <v>120</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E48">
+      <c r="F48">
         <v>1</v>
       </c>
-      <c r="F48" t="s">
+      <c r="G48" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>76</v>
       </c>
@@ -1689,11 +1815,11 @@
       <c r="C49" t="s">
         <v>122</v>
       </c>
-      <c r="E49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>77</v>
       </c>
@@ -1703,11 +1829,11 @@
       <c r="C50" t="s">
         <v>123</v>
       </c>
-      <c r="E50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>78</v>
       </c>
@@ -1717,11 +1843,11 @@
       <c r="C51" t="s">
         <v>124</v>
       </c>
-      <c r="E51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>79</v>
       </c>
@@ -1731,17 +1857,17 @@
       <c r="C52" t="s">
         <v>125</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E52">
+      <c r="F52">
         <v>2</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="G52" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>80</v>
       </c>
@@ -1751,17 +1877,18 @@
       <c r="C53" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" s="1"/>
+      <c r="E53" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E53">
+      <c r="F53">
         <v>2</v>
       </c>
-      <c r="F53" s="1" t="s">
+      <c r="G53" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>81</v>
       </c>
@@ -1771,17 +1898,17 @@
       <c r="C54" t="s">
         <v>127</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>121</v>
       </c>
-      <c r="E54">
+      <c r="F54">
         <v>1</v>
       </c>
-      <c r="F54" t="s">
+      <c r="G54" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="69" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="69" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>82</v>
       </c>
@@ -1791,17 +1918,18 @@
       <c r="C55" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="1"/>
+      <c r="E55" t="s">
         <v>121</v>
       </c>
-      <c r="E55">
+      <c r="F55">
         <v>1</v>
       </c>
-      <c r="F55" t="s">
+      <c r="G55" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="96.6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="96.6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>83</v>
       </c>
@@ -1811,17 +1939,18 @@
       <c r="C56" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" s="1"/>
+      <c r="E56" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E56">
+      <c r="F56">
         <v>2</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="G56" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="96.6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="96.6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>84</v>
       </c>
@@ -1831,17 +1960,18 @@
       <c r="C57" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D57" s="1"/>
+      <c r="E57" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E57">
+      <c r="F57">
         <v>2</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="G57" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>85</v>
       </c>
@@ -1851,17 +1981,18 @@
       <c r="C58" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="1"/>
+      <c r="E58" t="s">
         <v>121</v>
       </c>
-      <c r="E58">
+      <c r="F58">
         <v>1</v>
       </c>
-      <c r="F58" t="s">
+      <c r="G58" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>86</v>
       </c>
@@ -1871,17 +2002,18 @@
       <c r="C59" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="1"/>
+      <c r="E59" t="s">
         <v>121</v>
       </c>
-      <c r="E59">
+      <c r="F59">
         <v>1</v>
       </c>
-      <c r="F59" t="s">
+      <c r="G59" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>87</v>
       </c>
@@ -1891,17 +2023,17 @@
       <c r="C60" t="s">
         <v>129</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
         <v>117</v>
       </c>
-      <c r="E60">
+      <c r="F60">
         <v>1</v>
       </c>
-      <c r="F60" s="1" t="s">
+      <c r="G60" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>88</v>
       </c>
@@ -1911,17 +2043,17 @@
       <c r="C61" t="s">
         <v>131</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="E61" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E61" t="s">
+      <c r="F61" t="s">
         <v>132</v>
       </c>
-      <c r="F61" s="1" t="s">
+      <c r="G61" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>89</v>
       </c>
@@ -1931,11 +2063,11 @@
       <c r="C62" t="s">
         <v>134</v>
       </c>
-      <c r="E62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>90</v>
       </c>
@@ -1945,14 +2077,14 @@
       <c r="C63" t="s">
         <v>135</v>
       </c>
-      <c r="E63" t="s">
+      <c r="F63" t="s">
         <v>132</v>
       </c>
-      <c r="F63" s="1" t="s">
+      <c r="G63" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>91</v>
       </c>

</xml_diff>

<commit_message>
Updated document for recent code changes
</commit_message>
<xml_diff>
--- a/tests/docsrc/tables.xlsx
+++ b/tests/docsrc/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\metapp\tests\docsrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73BC5DFA-C6B2-48B2-A947-7C2D3D9BC272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01E63E8-77FF-4676-82FF-1D743214F08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="164">
   <si>
     <t>TypeKind</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -999,7 +999,8 @@
   <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1638,6 +1639,9 @@
       <c r="D40" s="1" t="s">
         <v>161</v>
       </c>
+      <c r="E40" t="s">
+        <v>114</v>
+      </c>
       <c r="F40">
         <v>1</v>
       </c>
@@ -1657,6 +1661,9 @@
       </c>
       <c r="D41" s="1" t="s">
         <v>162</v>
+      </c>
+      <c r="E41" t="s">
+        <v>114</v>
       </c>
       <c r="F41">
         <v>1</v>

</xml_diff>

<commit_message>
Added meta interface MetaPointerWrapper
</commit_message>
<xml_diff>
--- a/tests/docsrc/tables.xlsx
+++ b/tests/docsrc/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\metapp\tests\docsrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1892707-AA31-49BF-B215-9CD0A7A8909F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A71481-6C4F-4846-AF59-F0D779DEE5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="169">
   <si>
     <t>TypeKind</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -683,6 +683,11 @@
   </si>
   <si>
     <t>char32_t</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MetaAccessible
+MetaPointerWrapper</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1015,8 +1020,8 @@
   <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1664,8 +1669,8 @@
       <c r="D40" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E40" t="s">
-        <v>114</v>
+      <c r="E40" s="1" t="s">
+        <v>168</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -1674,7 +1679,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>69</v>
       </c>
@@ -1687,8 +1692,8 @@
       <c r="D41" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E41" t="s">
-        <v>114</v>
+      <c r="E41" s="1" t="s">
+        <v>168</v>
       </c>
       <c r="F41">
         <v>1</v>

</xml_diff>

<commit_message>
MetaCallable auxiliary functions use Variant of reference to pass the arguments to improve performance.
</commit_message>
<xml_diff>
--- a/tests/docsrc/tables.xlsx
+++ b/tests/docsrc/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\metapp\tests\docsrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A71481-6C4F-4846-AF59-F0D779DEE5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58792279-D74E-4856-B398-DEE3817808ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="171">
   <si>
     <t>TypeKind</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -688,6 +688,16 @@
   <si>
     <t>MetaAccessible
 MetaPointerWrapper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T[]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>char[] can cast to std::string.
+wchar_t[] can cast to std::wstring.
+T[] can cast to T *.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1020,8 +1030,8 @@
   <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1541,12 +1551,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>44</v>
       </c>
       <c r="B32">
         <v>50</v>
+      </c>
+      <c r="C32" t="s">
+        <v>169</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>170</v>
       </c>
       <c r="E32" t="s">
         <v>117</v>

</xml_diff>

<commit_message>
Removed cast to pointer ability from std::shared_ptr and std::unique_ptr
</commit_message>
<xml_diff>
--- a/tests/docsrc/tables.xlsx
+++ b/tests/docsrc/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\metapp\tests\docsrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58792279-D74E-4856-B398-DEE3817808ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB118671-E17C-475A-94EE-1B7605761D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="170">
   <si>
     <t>TypeKind</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -630,21 +630,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>All arithmetic types.
-Any types that can cast arithmetic types to.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Ditto</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Any pointers.
-char * can cast to std::string.
-wchar_t * can cast to std::wstring.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Use the cast rules of Variant</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -654,15 +643,6 @@
   </si>
   <si>
     <t>wchar_t *</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>T *
-std::weak_ptr&lt;T&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>T *</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -698,6 +678,20 @@
     <t>char[] can cast to std::string.
 wchar_t[] can cast to std::wstring.
 T[] can cast to T *.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>All arithmetic types.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cast to reference.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cast to pointer.
+char * can cast to std::string.
+wchar_t * can cast to std::wstring.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1029,9 +1023,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1081,7 +1075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1092,7 +1086,7 @@
         <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1109,7 +1103,7 @@
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -1126,7 +1120,7 @@
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1140,10 +1134,13 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D6" t="s">
-        <v>156</v>
+        <v>155</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1154,10 +1151,13 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D7" t="s">
-        <v>156</v>
+        <v>155</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1168,10 +1168,13 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D8" t="s">
-        <v>156</v>
+        <v>155</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1185,7 +1188,7 @@
         <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1202,7 +1205,7 @@
         <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1219,7 +1222,7 @@
         <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1236,7 +1239,7 @@
         <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1253,7 +1256,7 @@
         <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1270,7 +1273,7 @@
         <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1287,7 +1290,7 @@
         <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1304,7 +1307,7 @@
         <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1321,7 +1324,7 @@
         <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1338,7 +1341,7 @@
         <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -1355,7 +1358,7 @@
         <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1372,7 +1375,7 @@
         <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -1389,7 +1392,7 @@
         <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -1402,6 +1405,9 @@
       <c r="B22">
         <v>40</v>
       </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1414,7 +1420,7 @@
         <v>98</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="E23" t="s">
         <v>150</v>
@@ -1436,6 +1442,9 @@
       <c r="C24" t="s">
         <v>99</v>
       </c>
+      <c r="D24" t="s">
+        <v>168</v>
+      </c>
       <c r="F24">
         <v>1</v>
       </c>
@@ -1521,6 +1530,9 @@
       <c r="E29" t="s">
         <v>115</v>
       </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1559,10 +1571,10 @@
         <v>50</v>
       </c>
       <c r="C32" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E32" t="s">
         <v>117</v>
@@ -1616,7 +1628,7 @@
         <v>100</v>
       </c>
       <c r="D35" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -1629,6 +1641,9 @@
       <c r="B36">
         <v>54</v>
       </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -1637,6 +1652,9 @@
       <c r="B37">
         <v>55</v>
       </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -1649,7 +1667,7 @@
         <v>101</v>
       </c>
       <c r="D38" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -1666,7 +1684,7 @@
         <v>102</v>
       </c>
       <c r="D39" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -1683,10 +1701,10 @@
         <v>103</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -1705,11 +1723,9 @@
       <c r="C41" t="s">
         <v>108</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>162</v>
-      </c>
+      <c r="D41" s="1"/>
       <c r="E41" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -1729,7 +1745,7 @@
         <v>152</v>
       </c>
       <c r="D42" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -1749,7 +1765,7 @@
         <v>109</v>
       </c>
       <c r="D43" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E43" t="s">
         <v>115</v>
@@ -2146,6 +2162,9 @@
       </c>
       <c r="B64">
         <v>1024</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed casting to char * from std::string and std::wstring
</commit_message>
<xml_diff>
--- a/tests/docsrc/tables.xlsx
+++ b/tests/docsrc/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\metapp\tests\docsrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB118671-E17C-475A-94EE-1B7605761D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71858F6D-11E5-4FED-B94E-DF460489BC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="168">
   <si>
     <t>TypeKind</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -635,14 +635,6 @@
   </si>
   <si>
     <t>Use the cast rules of Variant</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>char *</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wchar_t *</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1023,9 +1015,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1086,7 +1078,7 @@
         <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1134,7 +1126,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D6" t="s">
         <v>155</v>
@@ -1151,7 +1143,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D7" t="s">
         <v>155</v>
@@ -1168,7 +1160,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D8" t="s">
         <v>155</v>
@@ -1420,7 +1412,7 @@
         <v>98</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E23" t="s">
         <v>150</v>
@@ -1443,7 +1435,7 @@
         <v>99</v>
       </c>
       <c r="D24" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -1571,10 +1563,10 @@
         <v>50</v>
       </c>
       <c r="C32" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E32" t="s">
         <v>117</v>
@@ -1666,9 +1658,6 @@
       <c r="C38" t="s">
         <v>101</v>
       </c>
-      <c r="D38" t="s">
-        <v>157</v>
-      </c>
       <c r="F38">
         <v>0</v>
       </c>
@@ -1683,9 +1672,6 @@
       <c r="C39" t="s">
         <v>102</v>
       </c>
-      <c r="D39" t="s">
-        <v>158</v>
-      </c>
       <c r="F39">
         <v>0</v>
       </c>
@@ -1704,7 +1690,7 @@
         <v>152</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -1725,7 +1711,7 @@
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -1745,7 +1731,7 @@
         <v>152</v>
       </c>
       <c r="D42" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -1765,7 +1751,7 @@
         <v>109</v>
       </c>
       <c r="D43" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E43" t="s">
         <v>115</v>

</xml_diff>